<commit_message>
Got credit checking done
</commit_message>
<xml_diff>
--- a/test_data/ec1_checklist.xlsx
+++ b/test_data/ec1_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aidan/Desktop/github-repos/ECE_Graduation_Validation/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017BE629-6C31-5D4B-9335-2AF6C2B1CA4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCAD329-76C5-CD40-8F1E-9E56CDB4C0E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3300" windowWidth="34560" windowHeight="20740" xr2:uid="{CCDFA643-959F-9442-8EA0-FAAE03167BCD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20740" xr2:uid="{CCDFA643-959F-9442-8EA0-FAAE03167BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1435,6 +1435,72 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1464,72 +1530,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1606,7 +1606,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1919,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608D3CE3-D47A-0540-A132-E9BE2E056D06}">
   <dimension ref="A4:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1933,17 +1933,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="22" thickBot="1">
       <c r="A5" s="3"/>
@@ -1960,19 +1960,19 @@
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="55"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="F6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="55"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" ht="17" thickBot="1"/>
     <row r="8" spans="1:9" ht="20" thickBot="1">
@@ -1991,21 +1991,21 @@
       <c r="E8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="10" spans="1:9" ht="20" thickBot="1">
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:9" ht="21" thickTop="1" thickBot="1">
       <c r="C11" s="4" t="s">
@@ -2247,13 +2247,13 @@
     </row>
     <row r="25" spans="3:7" ht="17" thickTop="1"/>
     <row r="26" spans="3:7" ht="20" thickBot="1">
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="3:7" ht="21" thickTop="1" thickBot="1">
       <c r="C27" s="4" t="s">
@@ -2359,13 +2359,13 @@
     </row>
     <row r="33" spans="3:8" ht="17" thickTop="1"/>
     <row r="34" spans="3:8" ht="20" thickBot="1">
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="3:8" ht="21" thickTop="1" thickBot="1">
       <c r="C35" s="4" t="s">
@@ -2392,7 +2392,7 @@
         <v>127</v>
       </c>
       <c r="E36" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>117</v>
@@ -2488,13 +2488,13 @@
     </row>
     <row r="42" spans="3:8" ht="17" thickTop="1"/>
     <row r="43" spans="3:8" ht="20" thickBot="1">
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
     </row>
     <row r="44" spans="3:8" ht="21" thickTop="1" thickBot="1">
       <c r="C44" s="4" t="s">
@@ -2818,13 +2818,13 @@
     </row>
     <row r="60" spans="3:8" ht="17" thickTop="1"/>
     <row r="61" spans="3:8" ht="20" thickBot="1">
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="34"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
     </row>
     <row r="62" spans="3:8" ht="21" thickTop="1" thickBot="1">
       <c r="C62" s="4" t="s">
@@ -2896,22 +2896,22 @@
     </row>
     <row r="66" spans="2:8" ht="17" thickTop="1"/>
     <row r="67" spans="2:8" ht="19">
-      <c r="C67" s="34" t="s">
+      <c r="C67" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="34"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
     </row>
     <row r="68" spans="2:8" ht="17" thickBot="1">
-      <c r="C68" s="43" t="s">
+      <c r="C68" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
     </row>
     <row r="69" spans="2:8" ht="17" thickBot="1">
       <c r="C69" s="1" t="s">
@@ -2929,43 +2929,43 @@
     </row>
     <row r="70" spans="2:8" ht="17" thickBot="1"/>
     <row r="71" spans="2:8" ht="17" thickBot="1">
-      <c r="C71" s="44" t="s">
+      <c r="C71" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
       <c r="F71" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="73" spans="2:8" ht="16" customHeight="1">
-      <c r="B73" s="47" t="s">
+      <c r="B73" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47"/>
-      <c r="F73" s="47"/>
-      <c r="G73" s="47"/>
-      <c r="H73" s="47"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="35"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="35"/>
     </row>
     <row r="74" spans="2:8">
-      <c r="B74" s="47"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
-      <c r="F74" s="47"/>
-      <c r="G74" s="47"/>
-      <c r="H74" s="47"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="35"/>
+      <c r="H74" s="35"/>
     </row>
     <row r="75" spans="2:8">
-      <c r="B75" s="47"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="47"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="35"/>
+      <c r="H75" s="35"/>
     </row>
     <row r="76" spans="2:8" ht="17" thickBot="1">
       <c r="B76" s="19"/>
@@ -2977,10 +2977,10 @@
       <c r="H76" s="19"/>
     </row>
     <row r="77" spans="2:8" ht="17" thickBot="1">
-      <c r="C77" s="44" t="s">
+      <c r="C77" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D77" s="44"/>
+      <c r="D77" s="32"/>
       <c r="E77" s="20" t="s">
         <v>92</v>
       </c>
@@ -2999,212 +2999,221 @@
       <c r="G78" s="18"/>
     </row>
     <row r="80" spans="2:8" ht="20" thickBot="1">
-      <c r="C80" s="34" t="s">
+      <c r="C80" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="34"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
     </row>
     <row r="81" spans="2:8" ht="17" thickTop="1">
-      <c r="C81" s="45" t="s">
+      <c r="C81" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="48" t="s">
+      <c r="D81" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="E81" s="48"/>
-      <c r="F81" s="48"/>
-      <c r="G81" s="49"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
+      <c r="G81" s="37"/>
     </row>
     <row r="82" spans="2:8">
-      <c r="C82" s="46"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="50"/>
-      <c r="F82" s="50"/>
-      <c r="G82" s="51"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="39"/>
     </row>
     <row r="83" spans="2:8">
       <c r="C83" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D83" s="39" t="s">
+      <c r="D83" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="40"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="30"/>
     </row>
     <row r="84" spans="2:8">
       <c r="C84" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D84" s="39" t="s">
+      <c r="D84" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E84" s="39"/>
-      <c r="F84" s="39"/>
-      <c r="G84" s="40"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="30"/>
     </row>
     <row r="85" spans="2:8">
       <c r="C85" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D85" s="39" t="s">
+      <c r="D85" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E85" s="39"/>
-      <c r="F85" s="39"/>
-      <c r="G85" s="40"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="30"/>
     </row>
     <row r="86" spans="2:8">
       <c r="C86" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D86" s="39" t="s">
+      <c r="D86" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E86" s="39"/>
-      <c r="F86" s="39"/>
-      <c r="G86" s="40"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="30"/>
     </row>
     <row r="87" spans="2:8">
       <c r="C87" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D87" s="39" t="s">
+      <c r="D87" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="E87" s="39"/>
-      <c r="F87" s="39"/>
-      <c r="G87" s="40"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="30"/>
     </row>
     <row r="88" spans="2:8" ht="17" thickBot="1">
       <c r="C88" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D88" s="41" t="s">
+      <c r="D88" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="E88" s="41"/>
-      <c r="F88" s="41"/>
-      <c r="G88" s="42"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="45"/>
     </row>
     <row r="89" spans="2:8" ht="17" thickTop="1"/>
     <row r="90" spans="2:8" ht="20" thickBot="1">
-      <c r="C90" s="34" t="s">
+      <c r="C90" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="34"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
     </row>
     <row r="91" spans="2:8" ht="17" thickTop="1">
       <c r="B91" s="7">
         <v>1</v>
       </c>
-      <c r="C91" s="35" t="s">
+      <c r="C91" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="D91" s="35"/>
-      <c r="E91" s="35"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="36"/>
+      <c r="D91" s="40"/>
+      <c r="E91" s="40"/>
+      <c r="F91" s="40"/>
+      <c r="G91" s="40"/>
+      <c r="H91" s="41"/>
     </row>
     <row r="92" spans="2:8">
-      <c r="B92" s="26">
+      <c r="B92" s="48">
         <v>2</v>
       </c>
-      <c r="C92" s="28" t="s">
+      <c r="C92" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="D92" s="29"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
-      <c r="G92" s="29"/>
-      <c r="H92" s="30"/>
+      <c r="D92" s="51"/>
+      <c r="E92" s="51"/>
+      <c r="F92" s="51"/>
+      <c r="G92" s="51"/>
+      <c r="H92" s="52"/>
     </row>
     <row r="93" spans="2:8" ht="19" customHeight="1">
-      <c r="B93" s="27"/>
-      <c r="C93" s="31"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="32"/>
-      <c r="H93" s="33"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="53"/>
+      <c r="D93" s="54"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="54"/>
+      <c r="G93" s="54"/>
+      <c r="H93" s="55"/>
     </row>
     <row r="94" spans="2:8">
       <c r="B94" s="9">
         <v>3</v>
       </c>
-      <c r="C94" s="37" t="s">
+      <c r="C94" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
-      <c r="G94" s="37"/>
-      <c r="H94" s="38"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="43"/>
     </row>
     <row r="95" spans="2:8">
       <c r="B95" s="9">
         <v>4</v>
       </c>
-      <c r="C95" s="37" t="s">
+      <c r="C95" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="37"/>
-      <c r="G95" s="37"/>
-      <c r="H95" s="38"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="42"/>
+      <c r="F95" s="42"/>
+      <c r="G95" s="42"/>
+      <c r="H95" s="43"/>
     </row>
     <row r="96" spans="2:8">
-      <c r="B96" s="26">
+      <c r="B96" s="48">
         <v>5</v>
       </c>
-      <c r="C96" s="28" t="s">
+      <c r="C96" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="29"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
-      <c r="G96" s="29"/>
-      <c r="H96" s="30"/>
+      <c r="D96" s="51"/>
+      <c r="E96" s="51"/>
+      <c r="F96" s="51"/>
+      <c r="G96" s="51"/>
+      <c r="H96" s="52"/>
     </row>
     <row r="97" spans="2:8">
-      <c r="B97" s="27"/>
-      <c r="C97" s="31"/>
-      <c r="D97" s="32"/>
-      <c r="E97" s="32"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="32"/>
-      <c r="H97" s="33"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="53"/>
+      <c r="D97" s="54"/>
+      <c r="E97" s="54"/>
+      <c r="F97" s="54"/>
+      <c r="G97" s="54"/>
+      <c r="H97" s="55"/>
     </row>
     <row r="98" spans="2:8" ht="17" thickBot="1">
       <c r="B98" s="11">
         <v>6</v>
       </c>
-      <c r="C98" s="24" t="s">
+      <c r="C98" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="D98" s="24"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="24"/>
-      <c r="H98" s="25"/>
+      <c r="D98" s="46"/>
+      <c r="E98" s="46"/>
+      <c r="F98" s="46"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="47"/>
     </row>
     <row r="99" spans="2:8" ht="17" thickTop="1"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C98:H98"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="C96:H97"/>
+    <mergeCell ref="C92:H93"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:H91"/>
+    <mergeCell ref="C94:H94"/>
+    <mergeCell ref="C95:H95"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="D87:G87"/>
+    <mergeCell ref="D88:G88"/>
     <mergeCell ref="D83:G83"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
@@ -3218,20 +3227,11 @@
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="C80:G80"/>
     <mergeCell ref="D81:G82"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:H91"/>
-    <mergeCell ref="C94:H94"/>
-    <mergeCell ref="C95:H95"/>
-    <mergeCell ref="D84:G84"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="D87:G87"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="C98:H98"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="C96:H97"/>
-    <mergeCell ref="C92:H93"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Make checklist correct again
</commit_message>
<xml_diff>
--- a/test_data/ec1_checklist.xlsx
+++ b/test_data/ec1_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aidan/Desktop/github-repos/ECE_Graduation_Validation/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCAD329-76C5-CD40-8F1E-9E56CDB4C0E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B55CD07-95DC-C747-A821-FF8EA6E49699}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20740" xr2:uid="{CCDFA643-959F-9442-8EA0-FAAE03167BCD}"/>
   </bookViews>
@@ -1435,6 +1435,90 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1446,90 +1530,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1606,7 +1606,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1920,7 +1920,7 @@
   <dimension ref="A4:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1933,17 +1933,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="1:9" ht="22" thickBot="1">
       <c r="A5" s="3"/>
@@ -1960,19 +1960,19 @@
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
       <c r="F6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55"/>
     </row>
     <row r="7" spans="1:9" ht="17" thickBot="1"/>
     <row r="8" spans="1:9" ht="20" thickBot="1">
@@ -1991,21 +1991,21 @@
       <c r="E8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="10" spans="1:9" ht="20" thickBot="1">
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:9" ht="21" thickTop="1" thickBot="1">
       <c r="C11" s="4" t="s">
@@ -2247,13 +2247,13 @@
     </row>
     <row r="25" spans="3:7" ht="17" thickTop="1"/>
     <row r="26" spans="3:7" ht="20" thickBot="1">
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="3:7" ht="21" thickTop="1" thickBot="1">
       <c r="C27" s="4" t="s">
@@ -2359,13 +2359,13 @@
     </row>
     <row r="33" spans="3:8" ht="17" thickTop="1"/>
     <row r="34" spans="3:8" ht="20" thickBot="1">
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
     </row>
     <row r="35" spans="3:8" ht="21" thickTop="1" thickBot="1">
       <c r="C35" s="4" t="s">
@@ -2392,7 +2392,7 @@
         <v>127</v>
       </c>
       <c r="E36" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>117</v>
@@ -2488,13 +2488,13 @@
     </row>
     <row r="42" spans="3:8" ht="17" thickTop="1"/>
     <row r="43" spans="3:8" ht="20" thickBot="1">
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
     </row>
     <row r="44" spans="3:8" ht="21" thickTop="1" thickBot="1">
       <c r="C44" s="4" t="s">
@@ -2818,13 +2818,13 @@
     </row>
     <row r="60" spans="3:8" ht="17" thickTop="1"/>
     <row r="61" spans="3:8" ht="20" thickBot="1">
-      <c r="C61" s="28" t="s">
+      <c r="C61" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
     </row>
     <row r="62" spans="3:8" ht="21" thickTop="1" thickBot="1">
       <c r="C62" s="4" t="s">
@@ -2896,22 +2896,22 @@
     </row>
     <row r="66" spans="2:8" ht="17" thickTop="1"/>
     <row r="67" spans="2:8" ht="19">
-      <c r="C67" s="28" t="s">
+      <c r="C67" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="34"/>
+      <c r="G67" s="34"/>
     </row>
     <row r="68" spans="2:8" ht="17" thickBot="1">
-      <c r="C68" s="31" t="s">
+      <c r="C68" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D68" s="31"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="43"/>
+      <c r="G68" s="43"/>
     </row>
     <row r="69" spans="2:8" ht="17" thickBot="1">
       <c r="C69" s="1" t="s">
@@ -2929,43 +2929,43 @@
     </row>
     <row r="70" spans="2:8" ht="17" thickBot="1"/>
     <row r="71" spans="2:8" ht="17" thickBot="1">
-      <c r="C71" s="32" t="s">
+      <c r="C71" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
       <c r="F71" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="73" spans="2:8" ht="16" customHeight="1">
-      <c r="B73" s="35" t="s">
+      <c r="B73" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="35"/>
-      <c r="H73" s="35"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
+      <c r="H73" s="47"/>
     </row>
     <row r="74" spans="2:8">
-      <c r="B74" s="35"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="35"/>
-      <c r="H74" s="35"/>
+      <c r="B74" s="47"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="47"/>
+      <c r="G74" s="47"/>
+      <c r="H74" s="47"/>
     </row>
     <row r="75" spans="2:8">
-      <c r="B75" s="35"/>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="35"/>
+      <c r="B75" s="47"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="47"/>
     </row>
     <row r="76" spans="2:8" ht="17" thickBot="1">
       <c r="B76" s="19"/>
@@ -2977,10 +2977,10 @@
       <c r="H76" s="19"/>
     </row>
     <row r="77" spans="2:8" ht="17" thickBot="1">
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D77" s="32"/>
+      <c r="D77" s="44"/>
       <c r="E77" s="20" t="s">
         <v>92</v>
       </c>
@@ -2999,221 +2999,212 @@
       <c r="G78" s="18"/>
     </row>
     <row r="80" spans="2:8" ht="20" thickBot="1">
-      <c r="C80" s="28" t="s">
+      <c r="C80" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
     </row>
     <row r="81" spans="2:8" ht="17" thickTop="1">
-      <c r="C81" s="33" t="s">
+      <c r="C81" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="36" t="s">
+      <c r="D81" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="37"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="49"/>
     </row>
     <row r="82" spans="2:8">
-      <c r="C82" s="34"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="39"/>
+      <c r="C82" s="46"/>
+      <c r="D82" s="50"/>
+      <c r="E82" s="50"/>
+      <c r="F82" s="50"/>
+      <c r="G82" s="51"/>
     </row>
     <row r="83" spans="2:8">
       <c r="C83" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D83" s="29" t="s">
+      <c r="D83" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="30"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="40"/>
     </row>
     <row r="84" spans="2:8">
       <c r="C84" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D84" s="29" t="s">
+      <c r="D84" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
-      <c r="G84" s="30"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="40"/>
     </row>
     <row r="85" spans="2:8">
       <c r="C85" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
-      <c r="G85" s="30"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="40"/>
     </row>
     <row r="86" spans="2:8">
       <c r="C86" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D86" s="29" t="s">
+      <c r="D86" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
-      <c r="G86" s="30"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="40"/>
     </row>
     <row r="87" spans="2:8">
       <c r="C87" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D87" s="29" t="s">
+      <c r="D87" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="30"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="40"/>
     </row>
     <row r="88" spans="2:8" ht="17" thickBot="1">
       <c r="C88" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D88" s="44" t="s">
+      <c r="D88" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="45"/>
+      <c r="E88" s="41"/>
+      <c r="F88" s="41"/>
+      <c r="G88" s="42"/>
     </row>
     <row r="89" spans="2:8" ht="17" thickTop="1"/>
     <row r="90" spans="2:8" ht="20" thickBot="1">
-      <c r="C90" s="28" t="s">
+      <c r="C90" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="28"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="34"/>
     </row>
     <row r="91" spans="2:8" ht="17" thickTop="1">
       <c r="B91" s="7">
         <v>1</v>
       </c>
-      <c r="C91" s="40" t="s">
+      <c r="C91" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="D91" s="40"/>
-      <c r="E91" s="40"/>
-      <c r="F91" s="40"/>
-      <c r="G91" s="40"/>
-      <c r="H91" s="41"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="35"/>
+      <c r="F91" s="35"/>
+      <c r="G91" s="35"/>
+      <c r="H91" s="36"/>
     </row>
     <row r="92" spans="2:8">
-      <c r="B92" s="48">
+      <c r="B92" s="26">
         <v>2</v>
       </c>
-      <c r="C92" s="50" t="s">
+      <c r="C92" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D92" s="51"/>
-      <c r="E92" s="51"/>
-      <c r="F92" s="51"/>
-      <c r="G92" s="51"/>
-      <c r="H92" s="52"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="30"/>
     </row>
     <row r="93" spans="2:8" ht="19" customHeight="1">
-      <c r="B93" s="49"/>
-      <c r="C93" s="53"/>
-      <c r="D93" s="54"/>
-      <c r="E93" s="54"/>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="55"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="31"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="32"/>
+      <c r="H93" s="33"/>
     </row>
     <row r="94" spans="2:8">
       <c r="B94" s="9">
         <v>3</v>
       </c>
-      <c r="C94" s="42" t="s">
+      <c r="C94" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D94" s="42"/>
-      <c r="E94" s="42"/>
-      <c r="F94" s="42"/>
-      <c r="G94" s="42"/>
-      <c r="H94" s="43"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="38"/>
     </row>
     <row r="95" spans="2:8">
       <c r="B95" s="9">
         <v>4</v>
       </c>
-      <c r="C95" s="42" t="s">
+      <c r="C95" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D95" s="42"/>
-      <c r="E95" s="42"/>
-      <c r="F95" s="42"/>
-      <c r="G95" s="42"/>
-      <c r="H95" s="43"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="37"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="38"/>
     </row>
     <row r="96" spans="2:8">
-      <c r="B96" s="48">
+      <c r="B96" s="26">
         <v>5</v>
       </c>
-      <c r="C96" s="50" t="s">
+      <c r="C96" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="D96" s="51"/>
-      <c r="E96" s="51"/>
-      <c r="F96" s="51"/>
-      <c r="G96" s="51"/>
-      <c r="H96" s="52"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="30"/>
     </row>
     <row r="97" spans="2:8">
-      <c r="B97" s="49"/>
-      <c r="C97" s="53"/>
-      <c r="D97" s="54"/>
-      <c r="E97" s="54"/>
-      <c r="F97" s="54"/>
-      <c r="G97" s="54"/>
-      <c r="H97" s="55"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="31"/>
+      <c r="D97" s="32"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="32"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="33"/>
     </row>
     <row r="98" spans="2:8" ht="17" thickBot="1">
       <c r="B98" s="11">
         <v>6</v>
       </c>
-      <c r="C98" s="46" t="s">
+      <c r="C98" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D98" s="46"/>
-      <c r="E98" s="46"/>
-      <c r="F98" s="46"/>
-      <c r="G98" s="46"/>
-      <c r="H98" s="47"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="25"/>
     </row>
     <row r="99" spans="2:8" ht="17" thickTop="1"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C98:H98"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="C96:H97"/>
-    <mergeCell ref="C92:H93"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:H91"/>
-    <mergeCell ref="C94:H94"/>
-    <mergeCell ref="C95:H95"/>
-    <mergeCell ref="D84:G84"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="D87:G87"/>
-    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C10:G10"/>
     <mergeCell ref="D83:G83"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
@@ -3227,11 +3218,20 @@
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="C80:G80"/>
     <mergeCell ref="D81:G82"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:H91"/>
+    <mergeCell ref="C94:H94"/>
+    <mergeCell ref="C95:H95"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="D87:G87"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="C98:H98"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="C96:H97"/>
+    <mergeCell ref="C92:H93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Worked on Excel spreadsheets
</commit_message>
<xml_diff>
--- a/test_data/ec1_checklist.xlsx
+++ b/test_data/ec1_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aidan/Desktop/github-repos/ECE_Graduation_Validation/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B55CD07-95DC-C747-A821-FF8EA6E49699}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D226F76-7594-6541-95DE-D751FE31104C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20740" xr2:uid="{CCDFA643-959F-9442-8EA0-FAAE03167BCD}"/>
   </bookViews>
@@ -1552,72 +1552,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>459078</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23662F40-F2F1-3446-8C05-A39D6FECFC2E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3048000" y="50800"/>
-          <a:ext cx="2757778" cy="368300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1919,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608D3CE3-D47A-0540-A132-E9BE2E056D06}">
   <dimension ref="A4:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2449,7 +2383,7 @@
         <v>114</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="3:8">
@@ -3234,6 +3168,5 @@
     <mergeCell ref="C92:H93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed color, fixed grade
</commit_message>
<xml_diff>
--- a/test_data/ec1_checklist.xlsx
+++ b/test_data/ec1_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aidan/Desktop/github-repos/ECE_Graduation_Validation/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EE7D5F-B1BA-C645-84B3-94B18368DAE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D43197C-C515-0C48-A28A-023484379AA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20740" xr2:uid="{CCDFA643-959F-9442-8EA0-FAAE03167BCD}"/>
   </bookViews>
@@ -448,7 +448,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE08D8E"/>
+        <fgColor rgb="FFDFC5FE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -759,15 +759,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,6 +815,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -843,6 +843,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -857,35 +884,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -901,6 +901,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDFC5FE"/>
       <color rgb="FFE08D8E"/>
       <color rgb="FFB31B1B"/>
     </mruColors>
@@ -1215,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608D3CE3-D47A-0540-A132-E9BE2E056D06}">
   <dimension ref="A2:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:M57"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1263,7 +1264,7 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="20" thickBot="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="29" t="s">
@@ -1271,7 +1272,7 @@
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="33"/>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="29" t="s">
@@ -1282,20 +1283,20 @@
       <c r="L4" s="31"/>
     </row>
     <row r="5" spans="1:12" ht="20" thickBot="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="29">
         <v>1234567</v>
       </c>
       <c r="E5" s="31"/>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="29" t="s">
@@ -1314,7 +1315,7 @@
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="13"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="32" t="s">
         <v>23</v>
       </c>
@@ -1324,260 +1325,260 @@
       <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:12" ht="21" thickTop="1" thickBot="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="17" thickTop="1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>4</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="3">
         <v>4</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="4">
         <v>3</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="4">
         <v>4</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="4">
         <v>4</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>4</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="4">
         <v>4</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K12" s="11" t="s">
-        <v>83</v>
+      <c r="K12" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="4">
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="4">
         <v>4</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="17" thickBot="1">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="5">
         <v>4</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="9" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" thickTop="1">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="4">
         <v>3</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20" thickBot="1">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="4">
         <v>1</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G16" s="32" t="s">
@@ -1590,197 +1591,197 @@
       <c r="L16" s="32"/>
     </row>
     <row r="17" spans="1:12" ht="21" thickTop="1" thickBot="1">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>4</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17" thickTop="1">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="4">
         <v>4</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="3">
         <v>3</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>4</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="4">
         <v>3</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17" thickBot="1">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="4">
         <v>3</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" thickTop="1">
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="4">
         <v>3</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L22" s="11" t="s">
+      <c r="L22" s="8" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1792,252 +1793,252 @@
       <c r="C23" s="32"/>
       <c r="D23" s="32"/>
       <c r="E23" s="32"/>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="4">
         <v>3</v>
       </c>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="K23" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="L23" s="11" t="s">
+      <c r="L23" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="21" thickTop="1" thickBot="1">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="4">
         <v>3</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L24" s="11" t="s">
+      <c r="L24" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" thickTop="1">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="3">
         <v>4</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="4">
         <v>3</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L25" s="11" t="s">
+      <c r="L25" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="4">
         <v>4</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="L26" s="11" t="s">
+      <c r="L26" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="4">
         <v>4</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="4">
         <v>4</v>
       </c>
-      <c r="J27" s="7" t="s">
+      <c r="J27" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K27" s="7" t="s">
+      <c r="K27" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="L27" s="11" t="s">
+      <c r="L27" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="4">
         <v>4</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="H28" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="7" t="s">
+      <c r="J28" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="K28" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="L28" s="11" t="s">
+      <c r="L28" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17" thickBot="1">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="5">
         <v>4</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H29" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="4">
         <v>3</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K29" s="7" t="s">
+      <c r="K29" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L29" s="11" t="s">
+      <c r="L29" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="17" thickTop="1">
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="H30" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="4">
         <v>3</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="J30" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="K30" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L30" s="11" t="s">
+      <c r="L30" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2049,205 +2050,205 @@
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="32"/>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="4">
         <v>4</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L31" s="11" t="s">
+      <c r="L31" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="21" thickTop="1" thickBot="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="G32" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="5">
         <v>3</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K32" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="L32" s="12" t="s">
+      <c r="L32" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="17" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="3">
         <v>2</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="16" customHeight="1" thickBot="1">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="4">
         <v>3</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="36" t="s">
+      <c r="G34" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37" t="s">
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="K34" s="38"/>
-      <c r="L34" s="20"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="17"/>
     </row>
     <row r="35" spans="1:13" ht="17" thickBot="1">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="5">
         <v>1</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
     </row>
     <row r="36" spans="1:13" ht="17" thickTop="1">
-      <c r="A36" s="27"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="G36" s="48" t="s">
+      <c r="A36" s="24"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="G36" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="27"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
     </row>
     <row r="38" spans="1:13" ht="17" thickBot="1">
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
     </row>
     <row r="39" spans="1:13" ht="21" thickTop="1" thickBot="1">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="42"/>
     </row>
     <row r="40" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="41"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="36"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
     </row>
     <row r="41" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A41" s="39"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="47"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="29" t="s">
         <v>114</v>
       </c>
@@ -2264,10 +2265,10 @@
       <c r="K42" s="31"/>
     </row>
     <row r="43" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="35"/>
+      <c r="B43" s="44"/>
       <c r="C43" s="29" t="s">
         <v>106</v>
       </c>
@@ -2285,799 +2286,799 @@
     </row>
     <row r="44" spans="1:13" ht="17" thickTop="1"/>
     <row r="45" spans="1:13" ht="19">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="17"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="14"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="26"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
     </row>
     <row r="47" spans="1:13" ht="16" customHeight="1">
-      <c r="A47" s="26"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
     </row>
     <row r="48" spans="1:13" ht="16" customHeight="1">
-      <c r="A48" s="23"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="23"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="23"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="25"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
     </row>
     <row r="51" spans="1:13" ht="16" customHeight="1">
-      <c r="A51" s="23"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="23"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
+      <c r="A52" s="20"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
     </row>
     <row r="53" spans="1:13" ht="17" customHeight="1">
-      <c r="A53" s="22"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="22"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
-      <c r="J56" s="25"/>
-      <c r="K56" s="25"/>
-      <c r="L56" s="25"/>
-      <c r="M56" s="25"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
-      <c r="L57" s="25"/>
-      <c r="M57" s="25"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="22"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="B58" s="17"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="17"/>
-      <c r="K58" s="17"/>
-      <c r="L58" s="17"/>
-      <c r="M58" s="17"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="17"/>
-      <c r="M59" s="17"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="14"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
-      <c r="K60" s="17"/>
-      <c r="L60" s="17"/>
-      <c r="M60" s="17"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="24"/>
-      <c r="J61" s="24"/>
-      <c r="K61" s="24"/>
-      <c r="L61" s="24"/>
-      <c r="M61" s="24"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="21"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-      <c r="K62" s="17"/>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="17"/>
-      <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="17"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="24"/>
-      <c r="J64" s="24"/>
-      <c r="K64" s="24"/>
-      <c r="L64" s="24"/>
-      <c r="M64" s="24"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="21"/>
     </row>
     <row r="65" spans="2:13">
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
     </row>
     <row r="66" spans="2:13" ht="19">
-      <c r="B66" s="17"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="20"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
-      <c r="J66" s="17"/>
-      <c r="K66" s="17"/>
-      <c r="L66" s="17"/>
-      <c r="M66" s="17"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
     </row>
     <row r="67" spans="2:13">
-      <c r="B67" s="17"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="21"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="17"/>
-      <c r="L67" s="17"/>
-      <c r="M67" s="17"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
     </row>
     <row r="68" spans="2:13">
-      <c r="B68" s="17"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="17"/>
-      <c r="K68" s="17"/>
-      <c r="L68" s="17"/>
-      <c r="M68" s="17"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="14"/>
     </row>
     <row r="69" spans="2:13">
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17"/>
-      <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
-      <c r="M69" s="17"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="14"/>
     </row>
     <row r="70" spans="2:13">
-      <c r="B70" s="17"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="17"/>
-      <c r="K70" s="17"/>
-      <c r="L70" s="17"/>
-      <c r="M70" s="17"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
     </row>
     <row r="71" spans="2:13">
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
-      <c r="J71" s="17"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
-      <c r="M71" s="17"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
     </row>
     <row r="72" spans="2:13" ht="16" customHeight="1">
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="17"/>
-      <c r="J72" s="17"/>
-      <c r="K72" s="17"/>
-      <c r="L72" s="17"/>
-      <c r="M72" s="17"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
     </row>
     <row r="73" spans="2:13">
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="M73" s="17"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
     </row>
     <row r="74" spans="2:13">
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="19"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
-      <c r="M74" s="17"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
     </row>
     <row r="75" spans="2:13">
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="17"/>
-      <c r="K75" s="17"/>
-      <c r="L75" s="17"/>
-      <c r="M75" s="17"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
     </row>
     <row r="76" spans="2:13">
-      <c r="B76" s="17"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="21"/>
-      <c r="H76" s="17"/>
-      <c r="I76" s="17"/>
-      <c r="J76" s="17"/>
-      <c r="K76" s="17"/>
-      <c r="L76" s="17"/>
-      <c r="M76" s="17"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
     </row>
     <row r="77" spans="2:13">
-      <c r="B77" s="17"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="21"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="17"/>
-      <c r="J77" s="17"/>
-      <c r="K77" s="17"/>
-      <c r="L77" s="17"/>
-      <c r="M77" s="17"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
     </row>
     <row r="78" spans="2:13">
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="17"/>
-      <c r="K78" s="17"/>
-      <c r="L78" s="17"/>
-      <c r="M78" s="17"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
     </row>
     <row r="79" spans="2:13" ht="19">
-      <c r="B79" s="17"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="20"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="17"/>
-      <c r="K79" s="17"/>
-      <c r="L79" s="17"/>
-      <c r="M79" s="17"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
     </row>
     <row r="80" spans="2:13">
-      <c r="B80" s="17"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="19"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
-      <c r="M80" s="17"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
     </row>
     <row r="81" spans="2:13">
-      <c r="B81" s="17"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="19"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="17"/>
-      <c r="L81" s="17"/>
-      <c r="M81" s="17"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
     </row>
     <row r="82" spans="2:13">
-      <c r="B82" s="17"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="21"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="17"/>
-      <c r="K82" s="17"/>
-      <c r="L82" s="17"/>
-      <c r="M82" s="17"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
     </row>
     <row r="83" spans="2:13">
-      <c r="B83" s="17"/>
-      <c r="C83" s="23"/>
-      <c r="D83" s="21"/>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="17"/>
-      <c r="K83" s="17"/>
-      <c r="L83" s="17"/>
-      <c r="M83" s="17"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
     </row>
     <row r="84" spans="2:13">
-      <c r="B84" s="17"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
-      <c r="K84" s="17"/>
-      <c r="L84" s="17"/>
-      <c r="M84" s="17"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
     </row>
     <row r="85" spans="2:13">
-      <c r="B85" s="17"/>
-      <c r="C85" s="23"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
-      <c r="K85" s="17"/>
-      <c r="L85" s="17"/>
-      <c r="M85" s="17"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
     </row>
     <row r="86" spans="2:13">
-      <c r="B86" s="17"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="21"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="21"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="17"/>
-      <c r="K86" s="17"/>
-      <c r="L86" s="17"/>
-      <c r="M86" s="17"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="14"/>
     </row>
     <row r="87" spans="2:13">
-      <c r="B87" s="17"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="21"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="17"/>
-      <c r="L87" s="17"/>
-      <c r="M87" s="17"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="14"/>
     </row>
     <row r="88" spans="2:13">
-      <c r="B88" s="17"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="17"/>
-      <c r="J88" s="17"/>
-      <c r="K88" s="17"/>
-      <c r="L88" s="17"/>
-      <c r="M88" s="17"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="14"/>
     </row>
     <row r="89" spans="2:13" ht="19">
-      <c r="B89" s="17"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="20"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="17"/>
-      <c r="L89" s="17"/>
-      <c r="M89" s="17"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="17"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="14"/>
     </row>
     <row r="90" spans="2:13">
-      <c r="B90" s="17"/>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="24"/>
-      <c r="H90" s="24"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
-      <c r="L90" s="17"/>
-      <c r="M90" s="17"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="21"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="14"/>
     </row>
     <row r="91" spans="2:13">
-      <c r="B91" s="21"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
-      <c r="H91" s="25"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="17"/>
-      <c r="L91" s="17"/>
-      <c r="M91" s="17"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="14"/>
     </row>
     <row r="92" spans="2:13" ht="19" customHeight="1">
-      <c r="B92" s="21"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="25"/>
-      <c r="H92" s="25"/>
-      <c r="I92" s="17"/>
-      <c r="J92" s="17"/>
-      <c r="K92" s="17"/>
-      <c r="L92" s="17"/>
-      <c r="M92" s="17"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="14"/>
     </row>
     <row r="93" spans="2:13">
-      <c r="B93" s="17"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
-      <c r="H93" s="24"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="17"/>
-      <c r="L93" s="17"/>
-      <c r="M93" s="17"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="14"/>
     </row>
     <row r="94" spans="2:13">
-      <c r="B94" s="17"/>
-      <c r="C94" s="24"/>
-      <c r="D94" s="24"/>
-      <c r="E94" s="24"/>
-      <c r="F94" s="24"/>
-      <c r="G94" s="24"/>
-      <c r="H94" s="24"/>
-      <c r="I94" s="17"/>
-      <c r="J94" s="17"/>
-      <c r="K94" s="17"/>
-      <c r="L94" s="17"/>
-      <c r="M94" s="17"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="21"/>
+      <c r="H94" s="21"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="14"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="14"/>
     </row>
     <row r="95" spans="2:13">
-      <c r="B95" s="21"/>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="25"/>
-      <c r="H95" s="25"/>
-      <c r="I95" s="17"/>
-      <c r="J95" s="17"/>
-      <c r="K95" s="17"/>
-      <c r="L95" s="17"/>
-      <c r="M95" s="17"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="22"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="14"/>
     </row>
     <row r="96" spans="2:13">
-      <c r="B96" s="21"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="25"/>
-      <c r="H96" s="25"/>
-      <c r="I96" s="17"/>
-      <c r="J96" s="17"/>
-      <c r="K96" s="17"/>
-      <c r="L96" s="17"/>
-      <c r="M96" s="17"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="22"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="14"/>
+      <c r="L96" s="14"/>
+      <c r="M96" s="14"/>
     </row>
     <row r="97" spans="2:13">
-      <c r="B97" s="17"/>
-      <c r="C97" s="24"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="24"/>
-      <c r="H97" s="24"/>
-      <c r="I97" s="17"/>
-      <c r="J97" s="17"/>
-      <c r="K97" s="17"/>
-      <c r="L97" s="17"/>
-      <c r="M97" s="17"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+      <c r="K97" s="14"/>
+      <c r="L97" s="14"/>
+      <c r="M97" s="14"/>
     </row>
     <row r="98" spans="2:13">
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="17"/>
-      <c r="K98" s="17"/>
-      <c r="L98" s="17"/>
-      <c r="M98" s="17"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+      <c r="K98" s="14"/>
+      <c r="L98" s="14"/>
+      <c r="M98" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="J34:K34"/>
-    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="J43:K43"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="A40:E41"/>
     <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:E42"/>
     <mergeCell ref="G36:L40"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="G16:L16"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="I4:L4"/>
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>